<commit_message>
Improvements in project structure
</commit_message>
<xml_diff>
--- a/Phase 1/Sprint 1/Burdown_chart_Sprint1.xlsx
+++ b/Phase 1/Sprint 1/Burdown_chart_Sprint1.xlsx
@@ -413,11 +413,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1287009518"/>
-        <c:axId val="833643772"/>
+        <c:axId val="1584197570"/>
+        <c:axId val="1837790985"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1287009518"/>
+        <c:axId val="1584197570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -469,10 +469,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="833643772"/>
+        <c:crossAx val="1837790985"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="833643772"/>
+        <c:axId val="1837790985"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,7 +547,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1287009518"/>
+        <c:crossAx val="1584197570"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>